<commit_message>
Melhorando codigo, novos arquivos exemplo
</commit_message>
<xml_diff>
--- a/assets/arc/exemplos_tabela.xlsx
+++ b/assets/arc/exemplos_tabela.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Micejane\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Micejane\Desktop\climstat-jailson\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="exemplos" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="75">
   <si>
     <t xml:space="preserve">  \ hora</t>
   </si>
@@ -222,13 +223,40 @@
   </si>
   <si>
     <t>HOUR = está em UTC</t>
+  </si>
+  <si>
+    <t>EPI</t>
+  </si>
+  <si>
+    <t>EPF</t>
+  </si>
+  <si>
+    <t>SF</t>
+  </si>
+  <si>
+    <t>ZCIT</t>
+  </si>
+  <si>
+    <t>Setor 2, Bloco I, Sala 18 </t>
+  </si>
+  <si>
+    <t>Tel.: (84) 3342-2244 ou (84) 9 9480-6848 </t>
+  </si>
+  <si>
+    <t>E-mail: isf.ufrn@gmail.com</t>
+  </si>
+  <si>
+    <t>toefl itp</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,6 +278,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -564,15 +598,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -633,6 +661,13 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -967,519 +1002,526 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="49"/>
+      <c r="D1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="50"/>
+      <c r="F1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="G1" s="49"/>
+      <c r="H1" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2" t="s">
+      <c r="I1" s="49"/>
+      <c r="J1" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2" t="s">
+      <c r="K1" s="49"/>
+      <c r="L1" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2" t="s">
+      <c r="M1" s="49"/>
+      <c r="N1" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2" t="s">
+      <c r="O1" s="49"/>
+      <c r="P1" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2" t="s">
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2" t="s">
+      <c r="S1" s="49"/>
+      <c r="T1" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2" t="s">
+      <c r="U1" s="49"/>
+      <c r="V1" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2" t="s">
+      <c r="W1" s="49"/>
+      <c r="X1" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="Y1" s="2"/>
+      <c r="Y1" s="49"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="S2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="T2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="U2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="V2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="W2" s="5" t="s">
+      <c r="W2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="X2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="Y2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="6"/>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="6"/>
+      <c r="B4" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6"/>
-      <c r="W5" s="6"/>
-      <c r="X5" s="6"/>
-      <c r="Y5" s="6"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="6"/>
-      <c r="W6" s="6"/>
-      <c r="X6" s="6"/>
-      <c r="Y6" s="6"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6"/>
-      <c r="T7" s="6"/>
-      <c r="U7" s="6"/>
-      <c r="V7" s="6"/>
-      <c r="W7" s="6"/>
-      <c r="X7" s="6"/>
-      <c r="Y7" s="6"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="6"/>
-      <c r="V8" s="6"/>
-      <c r="W8" s="6"/>
-      <c r="X8" s="6"/>
-      <c r="Y8" s="6"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="6"/>
-      <c r="U9" s="6"/>
-      <c r="V9" s="6"/>
-      <c r="W9" s="6"/>
-      <c r="X9" s="6"/>
-      <c r="Y9" s="6"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
-      <c r="U10" s="6"/>
-      <c r="V10" s="6"/>
-      <c r="W10" s="6"/>
-      <c r="X10" s="6"/>
-      <c r="Y10" s="6"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="4"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="6"/>
-      <c r="U11" s="6"/>
-      <c r="V11" s="6"/>
-      <c r="W11" s="6"/>
-      <c r="X11" s="6"/>
-      <c r="Y11" s="6"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="4"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="6"/>
-      <c r="U12" s="6"/>
-      <c r="V12" s="6"/>
-      <c r="W12" s="6"/>
-      <c r="X12" s="6"/>
-      <c r="Y12" s="6"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6"/>
-      <c r="S13" s="6"/>
-      <c r="T13" s="6"/>
-      <c r="U13" s="6"/>
-      <c r="V13" s="6"/>
-      <c r="W13" s="6"/>
-      <c r="X13" s="6"/>
-      <c r="Y13" s="6"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4"/>
+      <c r="X13" s="4"/>
+      <c r="Y13" s="4"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6"/>
-      <c r="U14" s="6"/>
-      <c r="V14" s="6"/>
-      <c r="W14" s="6"/>
-      <c r="X14" s="6"/>
-      <c r="Y14" s="6"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
+      <c r="Y14" s="4"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
-      <c r="S15" s="6"/>
-      <c r="T15" s="6"/>
-      <c r="U15" s="6"/>
-      <c r="V15" s="6"/>
-      <c r="W15" s="6"/>
-      <c r="X15" s="6"/>
-      <c r="Y15" s="6"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="4"/>
+      <c r="W15" s="4"/>
+      <c r="X15" s="4"/>
+      <c r="Y15" s="4"/>
     </row>
     <row r="16" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="5" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1489,127 +1531,127 @@
       </c>
     </row>
     <row r="18" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="8"/>
-      <c r="R18" s="8"/>
-      <c r="S18" s="8"/>
-      <c r="T18" s="8"/>
-      <c r="U18" s="8"/>
-      <c r="V18" s="8"/>
-      <c r="W18" s="8"/>
-      <c r="X18" s="8"/>
-      <c r="Y18" s="8"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
+      <c r="V18" s="6"/>
+      <c r="W18" s="6"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="6"/>
     </row>
     <row r="19" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="10" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="14">
+      <c r="C21" s="12">
         <v>0.1</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B22" s="15"/>
-      <c r="C22" s="16">
+      <c r="B22" s="13"/>
+      <c r="C22" s="14">
         <v>0.2</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B23" s="15"/>
-      <c r="C23" s="16">
+      <c r="B23" s="13"/>
+      <c r="C23" s="14">
         <v>0.3</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B24" s="15"/>
-      <c r="C24" s="16">
+      <c r="B24" s="13"/>
+      <c r="C24" s="14">
         <v>0.4</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="6" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B25" s="15"/>
-      <c r="C25" s="16">
+      <c r="B25" s="13"/>
+      <c r="C25" s="14">
         <v>0.5</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B26" s="15"/>
-      <c r="C26" s="16">
+      <c r="B26" s="13"/>
+      <c r="C26" s="14">
         <v>0.6</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B27" s="15"/>
-      <c r="C27" s="16">
+      <c r="B27" s="13"/>
+      <c r="C27" s="14">
         <v>0.7</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B28" s="15"/>
-      <c r="C28" s="16">
+      <c r="B28" s="13"/>
+      <c r="C28" s="14">
         <v>0.8</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B29" s="15"/>
-      <c r="C29" s="16">
+      <c r="B29" s="13"/>
+      <c r="C29" s="14">
         <v>0.9</v>
       </c>
     </row>
     <row r="30" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="17"/>
-      <c r="C30" s="18">
+      <c r="B30" s="15"/>
+      <c r="C30" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="5" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1624,423 +1666,418 @@
       </c>
     </row>
     <row r="36" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
-      <c r="S36" s="8"/>
-      <c r="T36" s="8"/>
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
+      <c r="P36" s="6"/>
+      <c r="Q36" s="6"/>
+      <c r="R36" s="6"/>
+      <c r="S36" s="6"/>
+      <c r="T36" s="6"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="19" t="s">
+      <c r="B37" s="17" t="s">
         <v>45</v>
       </c>
       <c r="C37" t="s">
         <v>46</v>
       </c>
-      <c r="F37" s="19" t="s">
+      <c r="F37" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="G37" s="19" t="s">
+      <c r="G37" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="I37" s="20" t="s">
+      <c r="I37" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="J37" s="20"/>
+      <c r="J37" s="18"/>
       <c r="K37" t="s">
         <v>50</v>
       </c>
-      <c r="O37" s="21" t="s">
+      <c r="O37" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="P37" s="22"/>
-      <c r="Q37" s="22"/>
-      <c r="R37" s="22"/>
-      <c r="S37" s="22"/>
-      <c r="T37" s="22"/>
-      <c r="U37" s="22"/>
-      <c r="V37" s="22"/>
-      <c r="W37" s="22"/>
-      <c r="X37" s="22"/>
-      <c r="Y37" s="22"/>
-      <c r="Z37" s="23"/>
+      <c r="P37" s="20"/>
+      <c r="Q37" s="20"/>
+      <c r="R37" s="20"/>
+      <c r="S37" s="20"/>
+      <c r="T37" s="20"/>
+      <c r="U37" s="20"/>
+      <c r="V37" s="20"/>
+      <c r="W37" s="20"/>
+      <c r="X37" s="20"/>
+      <c r="Y37" s="20"/>
+      <c r="Z37" s="21"/>
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A38" s="19">
+      <c r="A38" s="17">
         <v>22.1</v>
       </c>
-      <c r="B38" s="19">
+      <c r="B38" s="17">
         <v>0</v>
       </c>
       <c r="C38">
         <f>A38+B38</f>
         <v>22.1</v>
       </c>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E38" s="24"/>
-      <c r="F38" s="25">
+      <c r="E38" s="22"/>
+      <c r="F38" s="23">
         <v>1</v>
       </c>
-      <c r="G38" s="25">
+      <c r="G38" s="23">
         <v>4</v>
       </c>
-      <c r="I38" s="26" t="s">
+      <c r="I38" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="J38" s="26"/>
+      <c r="J38" s="24"/>
       <c r="K38" t="s">
         <v>54</v>
       </c>
-      <c r="O38" s="27" t="s">
+      <c r="O38" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="P38" s="28"/>
-      <c r="Q38" s="28"/>
-      <c r="R38" s="28"/>
-      <c r="S38" s="28"/>
-      <c r="T38" s="28"/>
-      <c r="U38" s="28"/>
-      <c r="V38" s="28"/>
-      <c r="W38" s="28"/>
-      <c r="X38" s="28"/>
-      <c r="Y38" s="28"/>
-      <c r="Z38" s="29"/>
+      <c r="P38" s="26"/>
+      <c r="Q38" s="26"/>
+      <c r="R38" s="26"/>
+      <c r="S38" s="26"/>
+      <c r="T38" s="26"/>
+      <c r="U38" s="26"/>
+      <c r="V38" s="26"/>
+      <c r="W38" s="26"/>
+      <c r="X38" s="26"/>
+      <c r="Y38" s="26"/>
+      <c r="Z38" s="27"/>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A39" s="19">
+      <c r="A39" s="17">
         <v>22.1</v>
       </c>
-      <c r="B39" s="19">
+      <c r="B39" s="17">
         <v>2.5</v>
       </c>
       <c r="C39">
         <f>A39+B39</f>
         <v>24.6</v>
       </c>
-      <c r="D39" s="19" t="s">
+      <c r="D39" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="E39" s="30"/>
-      <c r="F39" s="25">
+      <c r="E39" s="28"/>
+      <c r="F39" s="23">
         <v>2</v>
       </c>
-      <c r="G39" s="25">
+      <c r="G39" s="23">
         <v>5</v>
       </c>
-      <c r="I39" s="31" t="s">
+      <c r="I39" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="J39" s="31"/>
+      <c r="J39" s="29"/>
       <c r="K39" t="s">
         <v>58</v>
       </c>
-      <c r="O39" s="27" t="s">
+      <c r="O39" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="P39" s="28"/>
-      <c r="Q39" s="28"/>
-      <c r="R39" s="28"/>
-      <c r="S39" s="28"/>
-      <c r="T39" s="28"/>
-      <c r="U39" s="28"/>
-      <c r="V39" s="28"/>
-      <c r="W39" s="28"/>
-      <c r="X39" s="28"/>
-      <c r="Y39" s="28"/>
-      <c r="Z39" s="29"/>
+      <c r="P39" s="26"/>
+      <c r="Q39" s="26"/>
+      <c r="R39" s="26"/>
+      <c r="S39" s="26"/>
+      <c r="T39" s="26"/>
+      <c r="U39" s="26"/>
+      <c r="V39" s="26"/>
+      <c r="W39" s="26"/>
+      <c r="X39" s="26"/>
+      <c r="Y39" s="26"/>
+      <c r="Z39" s="27"/>
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A40" s="19">
+      <c r="A40" s="17">
         <v>22.1</v>
       </c>
-      <c r="B40" s="19">
+      <c r="B40" s="17">
         <v>6</v>
       </c>
       <c r="C40">
         <f>A40+B40</f>
         <v>28.1</v>
       </c>
-      <c r="D40" s="19" t="s">
+      <c r="D40" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="E40" s="30"/>
-      <c r="F40" s="25">
+      <c r="E40" s="28"/>
+      <c r="F40" s="23">
         <v>3</v>
       </c>
-      <c r="G40" s="25">
+      <c r="G40" s="23">
         <v>6</v>
       </c>
-      <c r="I40" s="32" t="s">
+      <c r="I40" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="J40" s="32"/>
+      <c r="J40" s="30"/>
       <c r="K40" t="s">
         <v>62</v>
       </c>
-      <c r="O40" s="27" t="s">
+      <c r="O40" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="P40" s="28"/>
-      <c r="Q40" s="28"/>
-      <c r="R40" s="28"/>
-      <c r="S40" s="28"/>
-      <c r="T40" s="28"/>
-      <c r="U40" s="28"/>
-      <c r="V40" s="28"/>
-      <c r="W40" s="28"/>
-      <c r="X40" s="28"/>
-      <c r="Y40" s="28"/>
-      <c r="Z40" s="29"/>
+      <c r="P40" s="26"/>
+      <c r="Q40" s="26"/>
+      <c r="R40" s="26"/>
+      <c r="S40" s="26"/>
+      <c r="T40" s="26"/>
+      <c r="U40" s="26"/>
+      <c r="V40" s="26"/>
+      <c r="W40" s="26"/>
+      <c r="X40" s="26"/>
+      <c r="Y40" s="26"/>
+      <c r="Z40" s="27"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="19"/>
-      <c r="B41" s="19"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="30"/>
-      <c r="F41" s="25">
+      <c r="A41" s="17"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="23">
         <v>4</v>
       </c>
-      <c r="G41" s="25">
+      <c r="G41" s="23">
         <v>7</v>
       </c>
-      <c r="O41" s="33" t="s">
+      <c r="O41" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="P41" s="34"/>
-      <c r="Q41" s="34"/>
-      <c r="R41" s="34"/>
-      <c r="S41" s="34"/>
-      <c r="T41" s="34"/>
-      <c r="U41" s="34"/>
-      <c r="V41" s="34"/>
-      <c r="W41" s="34"/>
-      <c r="X41" s="34"/>
-      <c r="Y41" s="34"/>
-      <c r="Z41" s="35"/>
+      <c r="P41" s="32"/>
+      <c r="Q41" s="32"/>
+      <c r="R41" s="32"/>
+      <c r="S41" s="32"/>
+      <c r="T41" s="32"/>
+      <c r="U41" s="32"/>
+      <c r="V41" s="32"/>
+      <c r="W41" s="32"/>
+      <c r="X41" s="32"/>
+      <c r="Y41" s="32"/>
+      <c r="Z41" s="33"/>
     </row>
     <row r="42" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="19"/>
-      <c r="B42" s="19"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="30"/>
-      <c r="F42" s="25">
+      <c r="A42" s="17"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="23">
         <v>5</v>
       </c>
-      <c r="G42" s="25">
+      <c r="G42" s="23">
         <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="19"/>
-      <c r="B43" s="19"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="36"/>
-      <c r="F43" s="25">
+      <c r="A43" s="17"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="34"/>
+      <c r="F43" s="23">
         <v>6</v>
       </c>
-      <c r="G43" s="25">
+      <c r="G43" s="23">
         <v>9</v>
       </c>
-      <c r="H43" s="37"/>
+      <c r="H43" s="35"/>
       <c r="K43" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="F44" s="38">
+      <c r="F44" s="36">
         <v>7</v>
       </c>
-      <c r="G44" s="38">
+      <c r="G44" s="36">
         <v>10</v>
       </c>
-      <c r="H44" s="39"/>
+      <c r="H44" s="37"/>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="F45" s="38">
+      <c r="F45" s="36">
         <v>8</v>
       </c>
-      <c r="G45" s="38">
+      <c r="G45" s="36">
         <v>11</v>
       </c>
-      <c r="H45" s="39"/>
+      <c r="H45" s="37"/>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="F46" s="38">
+      <c r="F46" s="36">
         <v>9</v>
       </c>
-      <c r="G46" s="38">
+      <c r="G46" s="36">
         <v>12</v>
       </c>
-      <c r="H46" s="39"/>
+      <c r="H46" s="37"/>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="F47" s="38">
+      <c r="F47" s="36">
         <v>10</v>
       </c>
-      <c r="G47" s="38">
+      <c r="G47" s="36">
         <v>13</v>
       </c>
-      <c r="H47" s="39"/>
+      <c r="H47" s="37"/>
     </row>
     <row r="48" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F48" s="38">
+      <c r="F48" s="36">
         <v>11</v>
       </c>
-      <c r="G48" s="38">
+      <c r="G48" s="36">
         <v>14</v>
       </c>
-      <c r="H48" s="39"/>
+      <c r="H48" s="37"/>
     </row>
     <row r="49" spans="5:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E49" s="40"/>
-      <c r="F49" s="38">
+      <c r="E49" s="38"/>
+      <c r="F49" s="36">
         <v>12</v>
       </c>
-      <c r="G49" s="38">
+      <c r="G49" s="36">
         <v>15</v>
       </c>
-      <c r="H49" s="41"/>
+      <c r="H49" s="39"/>
     </row>
     <row r="50" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E50" s="42"/>
-      <c r="F50" s="43">
+      <c r="E50" s="40"/>
+      <c r="F50" s="41">
         <v>13</v>
       </c>
-      <c r="G50" s="43">
+      <c r="G50" s="41">
         <v>16</v>
       </c>
     </row>
     <row r="51" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E51" s="42"/>
-      <c r="F51" s="43">
+      <c r="E51" s="40"/>
+      <c r="F51" s="41">
         <v>14</v>
       </c>
-      <c r="G51" s="43">
+      <c r="G51" s="41">
         <v>17</v>
       </c>
     </row>
     <row r="52" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E52" s="42"/>
-      <c r="F52" s="43">
+      <c r="E52" s="40"/>
+      <c r="F52" s="41">
         <v>15</v>
       </c>
-      <c r="G52" s="43">
+      <c r="G52" s="41">
         <v>18</v>
       </c>
     </row>
     <row r="53" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E53" s="42"/>
-      <c r="F53" s="43">
+      <c r="E53" s="40"/>
+      <c r="F53" s="41">
         <v>16</v>
       </c>
-      <c r="G53" s="43">
+      <c r="G53" s="41">
         <v>19</v>
       </c>
     </row>
     <row r="54" spans="5:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E54" s="42"/>
-      <c r="F54" s="43">
+      <c r="E54" s="40"/>
+      <c r="F54" s="41">
         <v>17</v>
       </c>
-      <c r="G54" s="43">
+      <c r="G54" s="41">
         <v>20</v>
       </c>
     </row>
     <row r="55" spans="5:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E55" s="44"/>
-      <c r="F55" s="43">
+      <c r="E55" s="42"/>
+      <c r="F55" s="41">
         <v>18</v>
       </c>
-      <c r="G55" s="43">
+      <c r="G55" s="41">
         <v>21</v>
       </c>
-      <c r="H55" s="45"/>
+      <c r="H55" s="43"/>
     </row>
     <row r="56" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="F56" s="46">
+      <c r="F56" s="44">
         <v>19</v>
       </c>
-      <c r="G56" s="46">
+      <c r="G56" s="44">
         <v>22</v>
       </c>
-      <c r="H56" s="47"/>
+      <c r="H56" s="45"/>
     </row>
     <row r="57" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="F57" s="46">
+      <c r="F57" s="44">
         <v>20</v>
       </c>
-      <c r="G57" s="46">
+      <c r="G57" s="44">
         <v>23</v>
       </c>
-      <c r="H57" s="47"/>
+      <c r="H57" s="45"/>
     </row>
     <row r="58" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="F58" s="46">
+      <c r="F58" s="44">
         <v>21</v>
       </c>
-      <c r="G58" s="46">
+      <c r="G58" s="44">
         <v>24</v>
       </c>
-      <c r="H58" s="47"/>
+      <c r="H58" s="45"/>
     </row>
     <row r="59" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="F59" s="46">
+      <c r="F59" s="44">
         <v>22</v>
       </c>
-      <c r="G59" s="46">
+      <c r="G59" s="44">
         <v>1</v>
       </c>
-      <c r="H59" s="47"/>
+      <c r="H59" s="45"/>
     </row>
     <row r="60" spans="5:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F60" s="46">
+      <c r="F60" s="44">
         <v>23</v>
       </c>
-      <c r="G60" s="46">
+      <c r="G60" s="44">
         <v>2</v>
       </c>
-      <c r="H60" s="47"/>
+      <c r="H60" s="45"/>
     </row>
     <row r="61" spans="5:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E61" s="48"/>
-      <c r="F61" s="25">
+      <c r="E61" s="46"/>
+      <c r="F61" s="23">
         <v>24</v>
       </c>
-      <c r="G61" s="25">
+      <c r="G61" s="23">
         <v>3</v>
       </c>
-      <c r="H61" s="49"/>
+      <c r="H61" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:W1"/>
     <mergeCell ref="X1:Y1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
@@ -2048,8 +2085,206 @@
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:W1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="17">
+        <v>1792</v>
+      </c>
+      <c r="D2" s="17">
+        <v>4636</v>
+      </c>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17">
+        <v>1414</v>
+      </c>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="17">
+        <v>273</v>
+      </c>
+      <c r="D4" s="17">
+        <v>290</v>
+      </c>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="48" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>